<commit_message>
DOCUMENTOS CORRETOS: GIT NAO BUGA ESSA MERDA
</commit_message>
<xml_diff>
--- a/Documentos/Estimativa de Tamanho e Esforço - LhamaTable.xlsx
+++ b/Documentos/Estimativa de Tamanho e Esforço - LhamaTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ian\Dropbox\ESO - TRABALHO\trabalho final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LhamaTable\LhamaTable\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -263,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="175">
   <si>
     <t>Estimativa de Esforço de Projeto baseado em                                                                Pontos de Caso de Uso (vs 1.1)</t>
   </si>
@@ -688,24 +688,6 @@
     <t>RFS17</t>
   </si>
   <si>
-    <t>RFS18</t>
-  </si>
-  <si>
-    <t>RFS19</t>
-  </si>
-  <si>
-    <t>RFS20</t>
-  </si>
-  <si>
-    <t>RFS21</t>
-  </si>
-  <si>
-    <t>RFS22</t>
-  </si>
-  <si>
-    <t>RFS23</t>
-  </si>
-  <si>
     <t>RFN1</t>
   </si>
   <si>
@@ -769,39 +751,12 @@
     <t>Usuário, Funcionalidades do Programa</t>
   </si>
   <si>
-    <t>Criar Tabuleiro</t>
-  </si>
-  <si>
-    <t>Tabuleiro, Cores</t>
-  </si>
-  <si>
-    <t>Consultar Tabuleiros</t>
-  </si>
-  <si>
-    <t>Alterar Tabuleiros</t>
-  </si>
-  <si>
-    <t>Tabuleiro, Mesa</t>
-  </si>
-  <si>
-    <t>Tabuleiro</t>
-  </si>
-  <si>
-    <t>Cancelar Tabuleiros</t>
-  </si>
-  <si>
     <t>Rolar Dados</t>
   </si>
   <si>
     <t>Funcionalidades do Progama</t>
   </si>
   <si>
-    <t>Exibir Tabuleiro</t>
-  </si>
-  <si>
-    <t>Tabuleiro, Funcionalidades do Progama</t>
-  </si>
-  <si>
     <t>Exibir Imagem</t>
   </si>
   <si>
@@ -814,15 +769,6 @@
     <t>Dados de Vídeo, Funcionalidades do Programa</t>
   </si>
   <si>
-    <t>Enviar Mensagem Privada</t>
-  </si>
-  <si>
-    <t>Ordenar Turnos</t>
-  </si>
-  <si>
-    <t>Mesa, Ficha, Funcionalidades do Programa</t>
-  </si>
-  <si>
     <t>Criptografar Senhas do Usuário</t>
   </si>
   <si>
@@ -836,6 +782,12 @@
   </si>
   <si>
     <t>Criar Log de Usuários</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>Mesa, Funcionalidades do Programa</t>
   </si>
 </sst>
 </file>
@@ -1830,49 +1782,15 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1886,6 +1804,50 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1897,11 +1859,14 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1909,24 +1874,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2568,7 +2520,7 @@
   </sheetPr>
   <dimension ref="A1:AMK37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B16" sqref="B16:D16"/>
     </sheetView>
   </sheetViews>
@@ -2614,32 +2566,32 @@
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="123" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-      <c r="J3" s="106"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
       <c r="K3" s="2"/>
       <c r="L3"/>
       <c r="M3"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
+      <c r="B4" s="123"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
       <c r="K4" s="2"/>
       <c r="L4"/>
       <c r="M4"/>
@@ -2659,54 +2611,54 @@
       <c r="M5"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="107" t="s">
+      <c r="B6" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="107"/>
-      <c r="D6" s="108" t="s">
+      <c r="C6" s="124"/>
+      <c r="D6" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="108"/>
-      <c r="H6" s="108"/>
-      <c r="I6" s="108"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="125"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="125"/>
+      <c r="I6" s="125"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="109" t="s">
+      <c r="B7" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="109"/>
-      <c r="D7" s="110" t="s">
+      <c r="C7" s="119"/>
+      <c r="D7" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="126"/>
+      <c r="G7" s="126"/>
+      <c r="H7" s="126"/>
+      <c r="I7" s="126"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="111" t="s">
+      <c r="B8" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="111"/>
+      <c r="C8" s="118"/>
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="109" t="s">
+      <c r="F8" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="109"/>
+      <c r="G8" s="119"/>
       <c r="H8" s="3" t="s">
         <v>8</v>
       </c>
@@ -2719,14 +2671,14 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="112" t="s">
+      <c r="D9" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="112"/>
-      <c r="H9" s="112"/>
-      <c r="I9" s="112"/>
+      <c r="E9" s="120"/>
+      <c r="F9" s="120"/>
+      <c r="G9" s="120"/>
+      <c r="H9" s="120"/>
+      <c r="I9" s="120"/>
       <c r="J9" s="6"/>
       <c r="K9"/>
       <c r="L9"/>
@@ -2761,18 +2713,18 @@
       <c r="M11"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="113" t="s">
+      <c r="B12" s="121" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="113"/>
-      <c r="D12" s="113"/>
-      <c r="E12" s="113"/>
+      <c r="C12" s="121"/>
+      <c r="D12" s="121"/>
+      <c r="E12" s="121"/>
       <c r="F12"/>
-      <c r="G12" s="114" t="s">
+      <c r="G12" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="114"/>
-      <c r="I12" s="114"/>
+      <c r="H12" s="122"/>
+      <c r="I12" s="122"/>
       <c r="J12" s="7" t="s">
         <v>12</v>
       </c>
@@ -2790,7 +2742,7 @@
       <c r="D13" s="115"/>
       <c r="E13" s="9">
         <f>Atores!D10+'RFS ou RFC'!D10</f>
-        <v>209</v>
+        <v>159</v>
       </c>
       <c r="F13"/>
       <c r="G13" s="115" t="s">
@@ -2800,7 +2752,7 @@
       <c r="I13" s="115"/>
       <c r="J13" s="10">
         <f t="shared" ref="J13:J20" si="0">$E$13*$E$14*K13</f>
-        <v>30.102913076923073</v>
+        <v>22.901259230769231</v>
       </c>
       <c r="K13" s="11">
         <f>dadoshistoricos!E31</f>
@@ -2820,14 +2772,14 @@
         <v>3.0864230769230767</v>
       </c>
       <c r="F14"/>
-      <c r="G14" s="117" t="s">
+      <c r="G14" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="117"/>
-      <c r="I14" s="117"/>
+      <c r="H14" s="114"/>
+      <c r="I14" s="114"/>
       <c r="J14" s="14">
         <f t="shared" si="0"/>
-        <v>106.07693179487178</v>
+        <v>80.699675384615389</v>
       </c>
       <c r="K14" s="15">
         <f>dadoshistoricos!F31*0.8</f>
@@ -2837,18 +2789,18 @@
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="118"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
+      <c r="B15" s="117"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="117"/>
       <c r="F15"/>
-      <c r="G15" s="117" t="s">
+      <c r="G15" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="117"/>
-      <c r="I15" s="117"/>
+      <c r="H15" s="114"/>
+      <c r="I15" s="114"/>
       <c r="J15" s="14">
         <f t="shared" si="0"/>
-        <v>26.519232948717946</v>
+        <v>20.174918846153847</v>
       </c>
       <c r="K15" s="16">
         <f>dadoshistoricos!F31*0.2</f>
@@ -2858,19 +2810,19 @@
       <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="119"/>
-      <c r="C16" s="119"/>
-      <c r="D16" s="119"/>
+      <c r="B16" s="113"/>
+      <c r="C16" s="113"/>
+      <c r="D16" s="113"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" s="117" t="s">
+      <c r="G16" s="114" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="117"/>
-      <c r="I16" s="117"/>
+      <c r="H16" s="114"/>
+      <c r="I16" s="114"/>
       <c r="J16" s="14">
         <f t="shared" si="0"/>
-        <v>43.004161538461531</v>
+        <v>32.716084615384617</v>
       </c>
       <c r="K16" s="16">
         <f>dadoshistoricos!G31</f>
@@ -2885,14 +2837,14 @@
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="G17" s="120" t="s">
+      <c r="G17" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="H17" s="120"/>
-      <c r="I17" s="120"/>
+      <c r="H17" s="109"/>
+      <c r="I17" s="109"/>
       <c r="J17" s="14">
         <f t="shared" si="0"/>
-        <v>358.36801282051277</v>
+        <v>272.63403846153847</v>
       </c>
       <c r="K17" s="16">
         <f>dadoshistoricos!H31</f>
@@ -2907,14 +2859,14 @@
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="G18" s="120" t="s">
+      <c r="G18" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="H18" s="120"/>
-      <c r="I18" s="120"/>
+      <c r="H18" s="109"/>
+      <c r="I18" s="109"/>
       <c r="J18" s="14">
         <f t="shared" si="0"/>
-        <v>14.33472051282051</v>
+        <v>10.905361538461538</v>
       </c>
       <c r="K18" s="16">
         <f>dadoshistoricos!I31</f>
@@ -2928,14 +2880,14 @@
       <c r="D19"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
-      <c r="G19" s="120" t="s">
+      <c r="G19" s="109" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="120"/>
-      <c r="I19" s="120"/>
+      <c r="H19" s="109"/>
+      <c r="I19" s="109"/>
       <c r="J19" s="14">
         <f t="shared" si="0"/>
-        <v>43.720897564102565</v>
+        <v>33.261352692307696</v>
       </c>
       <c r="K19" s="16">
         <f>dadoshistoricos!J31</f>
@@ -2951,14 +2903,14 @@
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
-      <c r="G20" s="120" t="s">
+      <c r="G20" s="109" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="120"/>
-      <c r="I20" s="120"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="109"/>
       <c r="J20" s="14">
         <f t="shared" si="0"/>
-        <v>22.935552820512818</v>
+        <v>17.44857846153846</v>
       </c>
       <c r="K20" s="16">
         <f>dadoshistoricos!K31</f>
@@ -2972,14 +2924,14 @@
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21" s="121" t="s">
+      <c r="G21" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="121"/>
-      <c r="I21" s="121"/>
+      <c r="H21" s="110"/>
+      <c r="I21" s="110"/>
       <c r="J21" s="18">
         <f>SUM(J13:J19)</f>
-        <v>622.12687025641014</v>
+        <v>473.29269076923077</v>
       </c>
       <c r="K21" s="19">
         <f>SUM(K13:K20)</f>
@@ -2988,31 +2940,31 @@
       <c r="L21" s="12"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="122" t="s">
+      <c r="B22" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="122"/>
-      <c r="D22" s="122"/>
-      <c r="E22" s="122"/>
-      <c r="F22" s="122"/>
-      <c r="G22" s="122"/>
-      <c r="H22" s="122"/>
-      <c r="I22" s="122"/>
-      <c r="J22" s="122"/>
+      <c r="C22" s="111"/>
+      <c r="D22" s="111"/>
+      <c r="E22" s="111"/>
+      <c r="F22" s="111"/>
+      <c r="G22" s="111"/>
+      <c r="H22" s="111"/>
+      <c r="I22" s="111"/>
+      <c r="J22" s="111"/>
       <c r="L22" s="12"/>
     </row>
     <row r="23" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="123" t="s">
+      <c r="B23" s="112" t="s">
         <v>115</v>
       </c>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
-      <c r="G23" s="123"/>
-      <c r="H23" s="123"/>
-      <c r="I23" s="123"/>
-      <c r="J23" s="123"/>
+      <c r="C23" s="112"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="112"/>
+      <c r="F23" s="112"/>
+      <c r="G23" s="112"/>
+      <c r="H23" s="112"/>
+      <c r="I23" s="112"/>
+      <c r="J23" s="112"/>
       <c r="L23" s="12"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
@@ -3070,47 +3022,47 @@
       <c r="L27" s="12"/>
     </row>
     <row r="28" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="123" t="s">
+      <c r="B28" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="123"/>
-      <c r="D28" s="123"/>
-      <c r="E28" s="123"/>
-      <c r="F28" s="123"/>
-      <c r="G28" s="123"/>
-      <c r="H28" s="123"/>
-      <c r="I28" s="123"/>
-      <c r="J28" s="123"/>
+      <c r="C28" s="112"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="112"/>
+      <c r="G28" s="112"/>
+      <c r="H28" s="112"/>
+      <c r="I28" s="112"/>
+      <c r="J28" s="112"/>
     </row>
     <row r="37" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B28:J28"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="B3:J4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G12:I12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="B3:J4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B28:J28"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.39374999999999999" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3156,11 +3108,11 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="127" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
       <c r="E2" s="21"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -3407,8 +3359,8 @@
   </sheetPr>
   <dimension ref="A1:AMK1011"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3439,11 +3391,11 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="B2" s="125" t="s">
+      <c r="B2" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
       <c r="E2" s="44"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
@@ -3502,7 +3454,7 @@
       </c>
       <c r="D7" s="9">
         <f>COUNTIF(CUC,B7)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="51"/>
       <c r="H7"/>
@@ -3518,7 +3470,7 @@
       </c>
       <c r="D8" s="27">
         <f>COUNTIF(CUC,B8)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E8" s="51"/>
       <c r="H8"/>
@@ -3534,7 +3486,7 @@
       </c>
       <c r="D9" s="27">
         <f>COUNTIF(CUC,B9)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="51"/>
       <c r="H9"/>
@@ -3548,16 +3500,16 @@
       </c>
       <c r="D10" s="57">
         <f>(C7*D7)+(C8*D8)+(C9*D9)</f>
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E10"/>
       <c r="H10"/>
       <c r="O10"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="126"/>
-      <c r="B11" s="126"/>
-      <c r="C11" s="126"/>
+      <c r="A11" s="129"/>
+      <c r="B11" s="129"/>
+      <c r="C11" s="129"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="H11"/>
@@ -3609,7 +3561,7 @@
         <v>125</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C14" s="64">
         <v>1</v>
@@ -3631,7 +3583,7 @@
         <v>126</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C15" s="64">
         <v>1</v>
@@ -3653,7 +3605,7 @@
         <v>127</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C16" s="64">
         <v>1</v>
@@ -3675,7 +3627,7 @@
         <v>128</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C17" s="64">
         <v>1</v>
@@ -3685,7 +3637,7 @@
         <v>Simples</v>
       </c>
       <c r="E17" s="63" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H17"/>
       <c r="O17" s="20">
@@ -3697,7 +3649,7 @@
         <v>129</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C18" s="64">
         <v>1</v>
@@ -3707,7 +3659,7 @@
         <v>Simples</v>
       </c>
       <c r="E18" s="63" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H18" s="43"/>
       <c r="O18" s="20">
@@ -3719,7 +3671,7 @@
         <v>130</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C19" s="64">
         <v>1</v>
@@ -3729,7 +3681,7 @@
         <v>Simples</v>
       </c>
       <c r="E19" s="63" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H19" s="43"/>
       <c r="O19" s="20">
@@ -3741,7 +3693,7 @@
         <v>131</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C20" s="64">
         <v>1</v>
@@ -3751,7 +3703,7 @@
         <v>Simples</v>
       </c>
       <c r="E20" s="63" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H20" s="43"/>
       <c r="O20" s="20">
@@ -3763,7 +3715,7 @@
         <v>132</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C21" s="64">
         <v>4</v>
@@ -3773,7 +3725,7 @@
         <v>Complexo</v>
       </c>
       <c r="E21" s="63" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H21" s="43"/>
       <c r="O21" s="20">
@@ -3785,7 +3737,7 @@
         <v>133</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C22" s="64">
         <v>1</v>
@@ -3795,7 +3747,7 @@
         <v>Simples</v>
       </c>
       <c r="E22" s="63" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="H22" s="43"/>
       <c r="O22" s="20">
@@ -3807,7 +3759,7 @@
         <v>134</v>
       </c>
       <c r="B23" s="63" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C23" s="64">
         <v>1</v>
@@ -3817,7 +3769,7 @@
         <v>Simples</v>
       </c>
       <c r="E23" s="63" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="O23" s="20">
         <v>11</v>
@@ -3828,7 +3780,7 @@
         <v>135</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C24" s="64">
         <v>1</v>
@@ -3838,7 +3790,7 @@
         <v>Simples</v>
       </c>
       <c r="E24" s="63" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="O24" s="20">
         <v>12</v>
@@ -3849,7 +3801,7 @@
         <v>136</v>
       </c>
       <c r="B25" s="63" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C25" s="64">
         <v>2</v>
@@ -3859,7 +3811,7 @@
         <v>Médio</v>
       </c>
       <c r="E25" s="63" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="O25" s="20">
         <v>13</v>
@@ -3870,7 +3822,7 @@
         <v>137</v>
       </c>
       <c r="B26" s="63" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C26" s="64">
         <v>2</v>
@@ -3880,7 +3832,7 @@
         <v>Médio</v>
       </c>
       <c r="E26" s="63" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="O26" s="20">
         <v>14</v>
@@ -3891,17 +3843,17 @@
         <v>138</v>
       </c>
       <c r="B27" s="63" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C27" s="64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" s="65" t="str">
         <f t="shared" si="0"/>
-        <v>Médio</v>
+        <v>Simples</v>
       </c>
       <c r="E27" s="63" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="O27" s="20">
         <v>15</v>
@@ -3912,17 +3864,17 @@
         <v>139</v>
       </c>
       <c r="B28" s="63" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C28" s="64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" s="65" t="str">
         <f t="shared" si="0"/>
-        <v>Simples</v>
+        <v>Médio</v>
       </c>
       <c r="E28" s="63" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="O28" s="20">
         <v>16</v>
@@ -3933,17 +3885,17 @@
         <v>140</v>
       </c>
       <c r="B29" s="63" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C29" s="64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="65" t="str">
         <f t="shared" si="0"/>
-        <v>Simples</v>
+        <v>Médio</v>
       </c>
       <c r="E29" s="63" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="O29" s="20">
         <v>17</v>
@@ -3954,17 +3906,17 @@
         <v>141</v>
       </c>
       <c r="B30" s="63" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C30" s="64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30" s="65" t="str">
         <f t="shared" si="0"/>
-        <v>Simples</v>
+        <v>Médio</v>
       </c>
       <c r="E30" s="63" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="O30" s="20">
         <v>18</v>
@@ -3975,7 +3927,7 @@
         <v>142</v>
       </c>
       <c r="B31" s="63" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C31" s="64">
         <v>2</v>
@@ -3985,7 +3937,7 @@
         <v>Médio</v>
       </c>
       <c r="E31" s="63" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="O31" s="20">
         <v>19</v>
@@ -3996,17 +3948,17 @@
         <v>143</v>
       </c>
       <c r="B32" s="63" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C32" s="64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="65" t="str">
         <f t="shared" si="0"/>
-        <v>Médio</v>
+        <v>Simples</v>
       </c>
       <c r="E32" s="63" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="O32" s="20">
         <v>21</v>
@@ -4017,17 +3969,17 @@
         <v>144</v>
       </c>
       <c r="B33" s="63" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="C33" s="64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" s="65" t="str">
         <f t="shared" si="0"/>
-        <v>Médio</v>
+        <v>Simples</v>
       </c>
       <c r="E33" s="63" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="O33" s="20">
         <v>22</v>
@@ -4037,144 +3989,79 @@
       <c r="A34" s="62" t="s">
         <v>145</v>
       </c>
-      <c r="B34" s="63" t="s">
-        <v>183</v>
+      <c r="B34" s="107" t="s">
+        <v>172</v>
       </c>
       <c r="C34" s="64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="65" t="str">
         <f t="shared" si="0"/>
-        <v>Médio</v>
+        <v>Simples</v>
       </c>
       <c r="E34" s="63" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="O34" s="20">
         <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="62" t="s">
-        <v>146</v>
-      </c>
-      <c r="B35" s="63" t="s">
-        <v>184</v>
-      </c>
-      <c r="C35" s="64">
-        <v>3</v>
-      </c>
-      <c r="D35" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>Complexo</v>
-      </c>
-      <c r="E35" s="63" t="s">
-        <v>185</v>
-      </c>
+      <c r="A35" s="106"/>
+      <c r="B35" s="107"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="63"/>
       <c r="O35" s="20">
         <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="62" t="s">
-        <v>147</v>
-      </c>
-      <c r="B36" s="63" t="s">
-        <v>186</v>
-      </c>
-      <c r="C36" s="64">
-        <v>2</v>
-      </c>
-      <c r="D36" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>Médio</v>
-      </c>
-      <c r="E36" s="63" t="s">
-        <v>167</v>
-      </c>
+      <c r="A36" s="62"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="63"/>
       <c r="O36" s="20">
         <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="62" t="s">
-        <v>148</v>
-      </c>
-      <c r="B37" s="63" t="s">
-        <v>187</v>
-      </c>
-      <c r="C37" s="64">
-        <v>2</v>
-      </c>
-      <c r="D37" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>Médio</v>
-      </c>
-      <c r="E37" s="63" t="s">
-        <v>167</v>
-      </c>
+      <c r="A37" s="62"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="63"/>
       <c r="O37" s="20">
         <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="62" t="s">
-        <v>149</v>
-      </c>
-      <c r="B38" s="63" t="s">
-        <v>188</v>
-      </c>
-      <c r="C38" s="64">
-        <v>1</v>
-      </c>
-      <c r="D38" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>Simples</v>
-      </c>
-      <c r="E38" s="63" t="s">
-        <v>176</v>
-      </c>
+      <c r="A38" s="62"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="63"/>
       <c r="O38" s="20">
         <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="62" t="s">
-        <v>150</v>
-      </c>
-      <c r="B39" s="63" t="s">
-        <v>189</v>
-      </c>
-      <c r="C39" s="64">
-        <v>1</v>
-      </c>
-      <c r="D39" s="65" t="str">
-        <f t="shared" si="0"/>
-        <v>Simples</v>
-      </c>
-      <c r="E39" s="63" t="s">
-        <v>176</v>
-      </c>
+      <c r="A39" s="62"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="63"/>
       <c r="O39" s="20">
         <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A40" s="134" t="s">
-        <v>151</v>
-      </c>
-      <c r="B40" s="135" t="s">
-        <v>190</v>
-      </c>
-      <c r="C40" s="136">
-        <v>1</v>
-      </c>
-      <c r="D40" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="135" t="s">
-        <v>176</v>
-      </c>
+      <c r="A40" s="106"/>
+      <c r="B40" s="107"/>
+      <c r="C40" s="108"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="107"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="66" t="s">
@@ -4182,7 +4069,7 @@
       </c>
       <c r="B41" s="66">
         <f>SUBTOTAL(103,B13:B40)</f>
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C41" s="67"/>
       <c r="D41" s="65"/>
@@ -9084,7 +8971,7 @@
   </sheetPr>
   <dimension ref="A1:AMK36"/>
   <sheetViews>
-    <sheetView topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -9142,12 +9029,12 @@
       <c r="M3"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="127" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="127"/>
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4"/>
@@ -9186,12 +9073,12 @@
       <c r="M6"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="127" t="s">
+      <c r="B7" s="132" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="127"/>
-      <c r="D7" s="127"/>
-      <c r="E7" s="127"/>
+      <c r="C7" s="132"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="132"/>
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" s="12"/>
@@ -9510,11 +9397,11 @@
       <c r="M21" s="12"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="128" t="s">
+      <c r="B22" s="131" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="128"/>
-      <c r="D22" s="128"/>
+      <c r="C22" s="131"/>
+      <c r="D22" s="131"/>
       <c r="E22" s="73">
         <f>0.6+(0.01*SUM(D9*E9,D10*E10,D11*E11,D12*E12,D13*E13,D14*E14,D15*E15,D16*E16,D17*E17,D18*E18,D19*E19,D20*E20,D21*E21))</f>
         <v>0.80499999999999994</v>
@@ -9561,12 +9448,12 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B26" s="129" t="s">
+      <c r="B26" s="133" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="129"/>
-      <c r="D26" s="129"/>
-      <c r="E26" s="129"/>
+      <c r="C26" s="133"/>
+      <c r="D26" s="133"/>
+      <c r="E26" s="133"/>
       <c r="F26" s="74"/>
       <c r="G26" s="75"/>
       <c r="I26"/>
@@ -9575,11 +9462,11 @@
       <c r="B27" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="130" t="s">
+      <c r="C27" s="134" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="130"/>
-      <c r="E27" s="130"/>
+      <c r="D27" s="134"/>
+      <c r="E27" s="134"/>
       <c r="F27" s="76" t="s">
         <v>32</v>
       </c>
@@ -9592,11 +9479,11 @@
       <c r="B28" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="131" t="s">
+      <c r="C28" s="130" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="131"/>
-      <c r="E28" s="131"/>
+      <c r="D28" s="130"/>
+      <c r="E28" s="130"/>
       <c r="F28" s="29">
         <v>1.5</v>
       </c>
@@ -9609,11 +9496,11 @@
       <c r="B29" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="C29" s="131" t="s">
+      <c r="C29" s="130" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="131"/>
-      <c r="E29" s="131"/>
+      <c r="D29" s="130"/>
+      <c r="E29" s="130"/>
       <c r="F29" s="29">
         <v>0.5</v>
       </c>
@@ -9626,11 +9513,11 @@
       <c r="B30" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="131" t="s">
+      <c r="C30" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="D30" s="131"/>
-      <c r="E30" s="131"/>
+      <c r="D30" s="130"/>
+      <c r="E30" s="130"/>
       <c r="F30" s="29">
         <v>1</v>
       </c>
@@ -9643,11 +9530,11 @@
       <c r="B31" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="131" t="s">
+      <c r="C31" s="130" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="131"/>
-      <c r="E31" s="131"/>
+      <c r="D31" s="130"/>
+      <c r="E31" s="130"/>
       <c r="F31" s="29">
         <v>0.5</v>
       </c>
@@ -9660,11 +9547,11 @@
       <c r="B32" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="131" t="s">
+      <c r="C32" s="130" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="131"/>
-      <c r="E32" s="131"/>
+      <c r="D32" s="130"/>
+      <c r="E32" s="130"/>
       <c r="F32" s="29">
         <v>1</v>
       </c>
@@ -9677,11 +9564,11 @@
       <c r="B33" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="131" t="s">
+      <c r="C33" s="130" t="s">
         <v>89</v>
       </c>
-      <c r="D33" s="131"/>
-      <c r="E33" s="131"/>
+      <c r="D33" s="130"/>
+      <c r="E33" s="130"/>
       <c r="F33" s="29">
         <v>2</v>
       </c>
@@ -9694,11 +9581,11 @@
       <c r="B34" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="C34" s="131" t="s">
+      <c r="C34" s="130" t="s">
         <v>91</v>
       </c>
-      <c r="D34" s="131"/>
-      <c r="E34" s="131"/>
+      <c r="D34" s="130"/>
+      <c r="E34" s="130"/>
       <c r="F34" s="29">
         <v>-1</v>
       </c>
@@ -9711,11 +9598,11 @@
       <c r="B35" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="131" t="s">
+      <c r="C35" s="130" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="131"/>
-      <c r="E35" s="131"/>
+      <c r="D35" s="130"/>
+      <c r="E35" s="130"/>
       <c r="F35" s="29">
         <v>-1</v>
       </c>
@@ -9725,13 +9612,13 @@
       <c r="I35" s="72"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="128" t="s">
+      <c r="B36" s="131" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="128"/>
-      <c r="D36" s="128"/>
-      <c r="E36" s="128"/>
-      <c r="F36" s="128"/>
+      <c r="C36" s="131"/>
+      <c r="D36" s="131"/>
+      <c r="E36" s="131"/>
+      <c r="F36" s="131"/>
       <c r="G36" s="77">
         <f>1.4+(-0.03*SUM(F28*G28,F29*G29,F30*G30,F31*G31,F32*G32,F33*G33,F34*G34,F35*G35))</f>
         <v>1.1599999999999999</v>
@@ -9741,6 +9628,11 @@
   </sheetData>
   <sheetProtection password="C6D5" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="14">
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="C27:E27"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E35"/>
@@ -9750,11 +9642,6 @@
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C32:E32"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="C27:E27"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" showErrorMessage="1" promptTitle="Influência" sqref="E9:E21 I9:I21">
@@ -9795,19 +9682,19 @@
   <sheetData>
     <row r="1" spans="1:55" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="78"/>
-      <c r="B1" s="132" t="s">
+      <c r="B1" s="135" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="132"/>
-      <c r="L1" s="132"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
+      <c r="K1" s="135"/>
+      <c r="L1" s="135"/>
       <c r="M1" s="79"/>
       <c r="N1" s="78"/>
       <c r="O1" s="78"/>
@@ -11602,10 +11489,10 @@
       <c r="G30" s="78"/>
       <c r="H30" s="78"/>
       <c r="I30" s="78"/>
-      <c r="J30" s="133" t="s">
+      <c r="J30" s="136" t="s">
         <v>112</v>
       </c>
-      <c r="K30" s="133"/>
+      <c r="K30" s="136"/>
       <c r="L30" s="100">
         <f>SUM(L5:L28)/4</f>
         <v>3.0864230769230767</v>

</xml_diff>